<commit_message>
Updated build arbwaves to include the scale and offset values to be used by the STM32 to restore the recovered A2D values to the correct scale/offset to match the gain values.
</commit_message>
<xml_diff>
--- a/weights/annsynth_gaintest.xlsx
+++ b/weights/annsynth_gaintest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24780" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="28100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +143,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -153,7 +159,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -187,8 +193,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -205,8 +215,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -223,6 +236,8 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -239,6 +254,8 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -279,100 +296,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
+                  <c:v>-0.358301101923702</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>-0.334848505251763</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>-0.310618808531788</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>-0.206554602026078</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-0.392346126210213</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-0.201050772086635</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>-0.487741317368602</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.339904187977856</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2.46125093176646</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>2.42394479968134</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>2.47271413199238</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2.82296154344147</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>2.11504419279044</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>1.58185755098179</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.928997303257867</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>0.585178238986637</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>0.428960737834263</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>0.225934425936663</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>0.189550248678271</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.0935633309570232</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>0.0759505745014086</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>0.00874464761597954</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>-0.0408384603702514</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>-0.0543419221770881</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>-0.118405673666667</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>-0.141863236573342</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>-0.187708530717087</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>-0.233058189109922</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>-0.25728690053321</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>-0.267970907829333</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>-0.301590012783648</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>-0.350007511310399</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-0.358301101923702</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -389,11 +406,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2145148568"/>
-        <c:axId val="-2145170232"/>
+        <c:axId val="2090031128"/>
+        <c:axId val="2126579512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2145148568"/>
+        <c:axId val="2090031128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -402,7 +419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145170232"/>
+        <c:crossAx val="2126579512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -410,7 +427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145170232"/>
+        <c:axId val="2126579512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -421,7 +438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145148568"/>
+        <c:crossAx val="2090031128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -803,7 +820,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -860,1154 +877,1154 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1">
-        <v>-0.33484850525176302</v>
-      </c>
-      <c r="C3" s="1">
+        <v>-0.35830110192370201</v>
+      </c>
+      <c r="C3" s="6">
         <v>9.2140184192298705E-2</v>
       </c>
       <c r="D3" s="1">
         <f>$B3*C3</f>
-        <v>-3.0853002950413346E-2</v>
-      </c>
-      <c r="E3" s="1">
+        <v>-3.3013929527553498E-2</v>
+      </c>
+      <c r="E3" s="6">
         <v>5.2694612616423803E-2</v>
       </c>
       <c r="F3" s="1">
         <f>$B3*E3</f>
-        <v>-1.7644712269430204E-2</v>
-      </c>
-      <c r="G3" s="1">
+        <v>-1.8880537765907261E-2</v>
+      </c>
+      <c r="G3" s="6">
         <v>-1.85246015691608E-4</v>
       </c>
       <c r="H3" s="1">
         <f>$B3*G3</f>
-        <v>6.2029351458179575E-5</v>
-      </c>
-      <c r="I3" s="1">
+        <v>6.6373851549278543E-5</v>
+      </c>
+      <c r="I3" s="6">
         <v>-0.209229427421179</v>
       </c>
       <c r="J3" s="1">
         <f>$B3*I3</f>
-        <v>7.0060161026664028E-2</v>
+        <v>7.4967134399873667E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>-0.31061880853178803</v>
-      </c>
-      <c r="C4" s="1">
+        <v>-0.33484850525176302</v>
+      </c>
+      <c r="C4" s="6">
         <v>-0.33054127615530998</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ref="D4:D34" si="0">$B4*C4</f>
-        <v>0.1026723373699391</v>
-      </c>
-      <c r="E4" s="1">
+        <v>0.11068125224461577</v>
+      </c>
+      <c r="E4" s="6">
         <v>-0.269402741302321</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4:F34" si="1">$B4*E4</f>
-        <v>8.3681558518524476E-2</v>
-      </c>
-      <c r="G4" s="1">
+        <v>9.0209105235809592E-2</v>
+      </c>
+      <c r="G4" s="6">
         <v>-0.37517662605394803</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" ref="H4:H34" si="2">$B4*G4</f>
-        <v>0.11653691657385351</v>
-      </c>
-      <c r="I4" s="1">
+        <v>0.12562733243956414</v>
+      </c>
+      <c r="I4" s="6">
         <v>0.38692795357410897</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" ref="J4:J34" si="3">$B4*I4</f>
-        <v>-0.12018709992683273</v>
+        <v>-0.12956224689441395</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>-0.206554602026078</v>
-      </c>
-      <c r="C5" s="1">
+        <v>-0.31061880853178803</v>
+      </c>
+      <c r="C5" s="6">
         <v>-2.8057249787680798E-2</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>5.7953540638406688E-3</v>
-      </c>
-      <c r="E5" s="1">
+        <v>8.7151094997281724E-3</v>
+      </c>
+      <c r="E5" s="6">
         <v>-3.8510836518481001E-2</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
-        <v>7.9545905107661942E-3</v>
-      </c>
-      <c r="G5" s="1">
+        <v>1.196219015493304E-2</v>
+      </c>
+      <c r="G5" s="6">
         <v>0.33615246902142898</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="2"/>
-        <v>-6.9433839458804783E-2</v>
-      </c>
-      <c r="I5" s="1">
+        <v>-0.10441527941245506</v>
+      </c>
+      <c r="I5" s="6">
         <v>0.18421656363451699</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>-3.8050778988139335E-2</v>
+        <v>-5.7221129507973978E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>-0.39234612621021298</v>
-      </c>
-      <c r="C6" s="1">
+        <v>-0.206554602026078</v>
+      </c>
+      <c r="C6" s="6">
         <v>-0.304528603084327</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>0.11948061774034321</v>
-      </c>
-      <c r="E6" s="1">
+        <v>6.2901784415640635E-2</v>
+      </c>
+      <c r="E6" s="6">
         <v>-0.25216139815349098</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>9.8934547745273341E-2</v>
-      </c>
-      <c r="G6" s="1">
+        <v>5.2085097241933727E-2</v>
+      </c>
+      <c r="G6" s="6">
         <v>-0.43806733368573902</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="2"/>
-        <v>0.17187402139083643</v>
-      </c>
-      <c r="I6" s="1">
+        <v>9.0484823770082934E-2</v>
+      </c>
+      <c r="I6" s="6">
         <v>2.0142848200709301E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>-7.9029684623886532E-3</v>
+        <v>-4.1605979937692113E-3</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>-0.20105077208663499</v>
-      </c>
-      <c r="C7" s="1">
+        <v>-0.39234612621021298</v>
+      </c>
+      <c r="C7" s="6">
         <v>8.5689018619407295E-2</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>-1.7227843352777879E-2</v>
-      </c>
-      <c r="E7" s="1">
+        <v>-3.3619754514079267E-2</v>
+      </c>
+      <c r="E7" s="6">
         <v>1.3476094152832E-2</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="1"/>
-        <v>-2.709379134139061E-3</v>
-      </c>
-      <c r="G7" s="1">
+        <v>-5.2872933373077366E-3</v>
+      </c>
+      <c r="G7" s="6">
         <v>0.16141117426354601</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="2"/>
-        <v>-3.2451841209096312E-2</v>
-      </c>
-      <c r="I7" s="1">
+        <v>-6.3329048949343908E-2</v>
+      </c>
+      <c r="I7" s="6">
         <v>-5.9550922683792695E-4</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>1.1972758984048027E-4</v>
+        <v>2.3364573827229965E-4</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>-0.48774131736860199</v>
-      </c>
-      <c r="C8" s="1">
+        <v>-0.20105077208663499</v>
+      </c>
+      <c r="C8" s="6">
         <v>-5.34365484360751E-2</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>2.6063212529842377E-2</v>
-      </c>
-      <c r="E8" s="1">
+        <v>1.0743459320717767E-2</v>
+      </c>
+      <c r="E8" s="6">
         <v>2.6721341130418401E-2</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
-        <v>-1.303310212480608E-2</v>
-      </c>
-      <c r="G8" s="1">
+        <v>-5.3723462654609753E-3</v>
+      </c>
+      <c r="G8" s="6">
         <v>0.17101184263361399</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="2"/>
-        <v>-8.3409541411750943E-2</v>
-      </c>
-      <c r="I8" s="1">
+        <v>-3.4382062997446214E-2</v>
+      </c>
+      <c r="I8" s="6">
         <v>7.5196225038837897E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>-3.6676305861588647E-2</v>
+        <v>-1.5118259102058714E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>0.33990418797785599</v>
-      </c>
-      <c r="C9" s="1">
+        <v>-0.48774131736860199</v>
+      </c>
+      <c r="C9" s="6">
         <v>-1.11644421443389E-2</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>-3.7948406412972673E-3</v>
-      </c>
-      <c r="E9" s="1">
+        <v>5.4453597191653951E-3</v>
+      </c>
+      <c r="E9" s="6">
         <v>-5.69024077897358E-2</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
-        <v>-1.9341366713754974E-2</v>
-      </c>
-      <c r="G9" s="1">
+        <v>2.775365533681114E-2</v>
+      </c>
+      <c r="G9" s="6">
         <v>-9.1145922246211403E-2</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="2"/>
-        <v>-3.0980880688591287E-2</v>
-      </c>
-      <c r="I9" s="1">
+        <v>4.4455632189143314E-2</v>
+      </c>
+      <c r="I9" s="6">
         <v>6.9489769521763403E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>2.3619863682063355E-2</v>
+        <v>-3.3893031730185409E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>2.4612509317664601</v>
-      </c>
-      <c r="C10" s="1">
+        <v>0.33990418797785599</v>
+      </c>
+      <c r="C10" s="6">
         <v>8.7048462945420402E-2</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>0.21424811053325415</v>
-      </c>
-      <c r="E10" s="1">
+        <v>2.9588137112183607E-2</v>
+      </c>
+      <c r="E10" s="6">
         <v>7.3715919049361894E-2</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
-        <v>0.18143337444626292</v>
-      </c>
-      <c r="G10" s="1">
+        <v>2.505634960551472E-2</v>
+      </c>
+      <c r="G10" s="6">
         <v>0.16485018506441901</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="2"/>
-        <v>0.40573767159167468</v>
-      </c>
-      <c r="I10" s="1">
+        <v>5.6033268292320623E-2</v>
+      </c>
+      <c r="I10" s="6">
         <v>0.68045234601643301</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>1.6747639706556194</v>
+        <v>0.23128860213034275</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
-        <v>2.4239447996813399</v>
-      </c>
-      <c r="C11" s="1">
+        <v>2.4612509317664601</v>
+      </c>
+      <c r="C11" s="6">
         <v>0.40049694623618198</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>0.97078249011745055</v>
-      </c>
-      <c r="E11" s="1">
+        <v>0.98572348209342475</v>
+      </c>
+      <c r="E11" s="6">
         <v>0.51027106144778001</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="1"/>
-        <v>1.2368688858242238</v>
-      </c>
-      <c r="G11" s="1">
+        <v>1.2559051254418092</v>
+      </c>
+      <c r="G11" s="6">
         <v>1.2290913744999299</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="2"/>
-        <v>2.9792496455522954</v>
-      </c>
-      <c r="I11" s="1">
+        <v>3.0251022907140714</v>
+      </c>
+      <c r="I11" s="6">
         <v>3.10802128193895E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>7.5336720236548499E-2</v>
+        <v>7.6496202761222293E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
-        <v>2.47271413199238</v>
-      </c>
-      <c r="C12" s="1">
+        <v>2.4239447996813399</v>
+      </c>
+      <c r="C12" s="6">
         <v>0.105880166628984</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>0.26181138432119672</v>
-      </c>
-      <c r="E12" s="1">
+        <v>0.25664767928971954</v>
+      </c>
+      <c r="E12" s="6">
         <v>0.15986792416277601</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="1"/>
-        <v>0.39530767532958233</v>
-      </c>
-      <c r="G12" s="1">
+        <v>0.38751102341021171</v>
+      </c>
+      <c r="G12" s="6">
         <v>0.153714610509424</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="2"/>
-        <v>0.38009228970035713</v>
-      </c>
-      <c r="I12" s="1">
+        <v>0.37259573077936098</v>
+      </c>
+      <c r="I12" s="6">
         <v>-2.3959078506738E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>-5.924395201312594E-2</v>
+        <v>-5.8075483751564537E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>2.8229615434414699</v>
-      </c>
-      <c r="C13" s="1">
+        <v>2.47271413199238</v>
+      </c>
+      <c r="C13" s="6">
         <v>0.142929396408674</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0.40348418948898801</v>
-      </c>
-      <c r="E13" s="1">
+        <v>0.35342353837686913</v>
+      </c>
+      <c r="E13" s="6">
         <v>7.9416823216849106E-2</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
-        <v>0.22419063784345472</v>
-      </c>
-      <c r="G13" s="1">
+        <v>0.19637510108624331</v>
+      </c>
+      <c r="G13" s="6">
         <v>-0.55870881231130898</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="2"/>
-        <v>-1.5772134911366833</v>
-      </c>
-      <c r="I13" s="1">
+        <v>-1.3815271758708518</v>
+      </c>
+      <c r="I13" s="6">
         <v>0.49823124742588598</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>1.406487651224148</v>
+        <v>1.2319834465101804</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1">
-        <v>2.1150441927904402</v>
-      </c>
-      <c r="C14" s="1">
+        <v>2.8229615434414699</v>
+      </c>
+      <c r="C14" s="6">
         <v>-0.18370831465875301</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>-0.38855120408631444</v>
-      </c>
-      <c r="E14" s="1">
+        <v>-0.51860150749210465</v>
+      </c>
+      <c r="E14" s="6">
         <v>-0.100559145964472</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="1"/>
-        <v>-0.21268703770412276</v>
-      </c>
-      <c r="G14" s="1">
+        <v>-0.28387460189902197</v>
+      </c>
+      <c r="G14" s="6">
         <v>1.38302135382219E-2</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="2"/>
-        <v>2.9251512829067957E-2</v>
-      </c>
-      <c r="I14" s="1">
+        <v>3.9042160955984007E-2</v>
+      </c>
+      <c r="I14" s="6">
         <v>-4.8950859808394198E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>-0.10353323176984311</v>
+        <v>-0.1381863947574915</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1">
-        <v>1.58185755098179</v>
-      </c>
-      <c r="C15" s="1">
+        <v>2.1150441927904402</v>
+      </c>
+      <c r="C15" s="6">
         <v>-0.31591768085737298</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>-0.49973676895289076</v>
-      </c>
-      <c r="E15" s="1">
+        <v>-0.66817985629721033</v>
+      </c>
+      <c r="E15" s="6">
         <v>-0.23528676947037799</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>-0.37219015293282914</v>
-      </c>
-      <c r="G15" s="1">
+        <v>-0.49764191540874603</v>
+      </c>
+      <c r="G15" s="6">
         <v>-0.193300256357374</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="2"/>
-        <v>-0.30577347012562783</v>
-      </c>
-      <c r="I15" s="1">
+        <v>-0.40883858467356726</v>
+      </c>
+      <c r="I15" s="6">
         <v>-0.32263502806037098</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>-0.51036265534851954</v>
+        <v>-0.68238734248986832</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1">
-        <v>0.928997303257867</v>
-      </c>
-      <c r="C16" s="1">
+        <v>1.58185755098179</v>
+      </c>
+      <c r="C16" s="6">
         <v>-8.7860418051233596E-2</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>-8.1622091432704824E-2</v>
-      </c>
-      <c r="E16" s="1">
+        <v>-0.13898266572676063</v>
+      </c>
+      <c r="E16" s="6">
         <v>-8.5817736659812294E-2</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="1"/>
-        <v>-7.9724445928659418E-2</v>
-      </c>
-      <c r="G16" s="1">
+        <v>-0.13575143474349086</v>
+      </c>
+      <c r="G16" s="6">
         <v>-0.18354331320626099</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="2"/>
-        <v>-0.1705112429996305</v>
-      </c>
-      <c r="I16" s="1">
+        <v>-0.29033937592753967</v>
+      </c>
+      <c r="I16" s="6">
         <v>-0.180834294205446</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>-0.16799457165339907</v>
+        <v>-0.28605409376534729</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
-        <v>0.58517823898663701</v>
-      </c>
-      <c r="C17" s="1">
+        <v>0.928997303257867</v>
+      </c>
+      <c r="C17" s="6">
         <v>-3.0147529534417999E-2</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>-1.7641678242748354E-2</v>
-      </c>
-      <c r="E17" s="1">
+        <v>-2.800697363736122E-2</v>
+      </c>
+      <c r="E17" s="6">
         <v>-8.8300513005802495E-2</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="1"/>
-        <v>-5.1671538702352145E-2</v>
-      </c>
-      <c r="G17" s="1">
+        <v>-8.2030938458676733E-2</v>
+      </c>
+      <c r="G17" s="6">
         <v>-0.12643888560755701</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="2"/>
-        <v>-7.3989284419263057E-2</v>
-      </c>
-      <c r="I17" s="1">
+        <v>-0.11746138375635039</v>
+      </c>
+      <c r="I17" s="6">
         <v>-0.41800478899680399</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>-0.24460730631313055</v>
+        <v>-0.38832532172690465</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1">
-        <v>0.42896073783426297</v>
-      </c>
-      <c r="C18" s="1">
+        <v>0.58517823898663701</v>
+      </c>
+      <c r="C18" s="6">
         <v>-0.38619071684934397</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>-0.16566065484443754</v>
-      </c>
-      <c r="E18" s="1">
+        <v>-0.22599040359888609</v>
+      </c>
+      <c r="E18" s="6">
         <v>-0.39901041946947002</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="1"/>
-        <v>-0.17115980393918262</v>
-      </c>
-      <c r="G18" s="1">
+        <v>-0.2334922146024638</v>
+      </c>
+      <c r="G18" s="6">
         <v>-4.2478079239865102E-2</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="2"/>
-        <v>-1.8221428212514823E-2</v>
-      </c>
-      <c r="I18" s="1">
+        <v>-2.4857247605119086E-2</v>
+      </c>
+      <c r="I18" s="6">
         <v>-2.1009541195469099E-2</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="3"/>
-        <v>-9.0122682927677687E-3</v>
+        <v>-1.2294326318681811E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
-        <v>0.22593442593666299</v>
-      </c>
-      <c r="C19" s="1">
+        <v>0.42896073783426297</v>
+      </c>
+      <c r="C19" s="6">
         <v>-8.0724437157012399E-2</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>-1.8238429368129822E-2</v>
-      </c>
-      <c r="E19" s="1">
+        <v>-3.4627614124127633E-2</v>
+      </c>
+      <c r="E19" s="6">
         <v>-9.8681591183171893E-2</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="1"/>
-        <v>-2.2295568654486404E-2</v>
-      </c>
-      <c r="G19" s="1">
+        <v>-4.2330528164592512E-2</v>
+      </c>
+      <c r="G19" s="6">
         <v>-0.56021245940201603</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="2"/>
-        <v>-0.12657128041756061</v>
-      </c>
-      <c r="I19" s="1">
+        <v>-0.24030914992903588</v>
+      </c>
+      <c r="I19" s="6">
         <v>-7.7840691690625893E-2</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="3"/>
-        <v>-1.7586891991634334E-2</v>
+        <v>-3.3390600541140264E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>0.189550248678271</v>
-      </c>
-      <c r="C20" s="1">
+        <v>0.22593442593666299</v>
+      </c>
+      <c r="C20" s="6">
         <v>0.108291602007242</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>2.0526700090241073E-2</v>
-      </c>
-      <c r="E20" s="1">
+        <v>2.4466800933267804E-2</v>
+      </c>
+      <c r="E20" s="6">
         <v>8.60592941715424E-2</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="1"/>
-        <v>1.631256061129234E-2</v>
-      </c>
-      <c r="G20" s="1">
+        <v>1.944375722516184E-2</v>
+      </c>
+      <c r="G20" s="6">
         <v>-3.1887935649155597E-2</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="2"/>
-        <v>-6.0443661321341463E-3</v>
-      </c>
-      <c r="I20" s="1">
+        <v>-7.2045824351972204E-3</v>
+      </c>
+      <c r="I20" s="6">
         <v>0.146549171624312</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="3"/>
-        <v>2.7778431924982954E-2</v>
+        <v>3.3110502962432432E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1">
-        <v>9.3563330957023197E-2</v>
-      </c>
-      <c r="C21" s="1">
+        <v>0.189550248678271</v>
+      </c>
+      <c r="C21" s="6">
         <v>6.9039965779375503E-2</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>6.4596091674772663E-3</v>
-      </c>
-      <c r="E21" s="1">
+        <v>1.3086542682219947E-2</v>
+      </c>
+      <c r="E21" s="6">
         <v>-1.6065674742171E-2</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="1"/>
-        <v>-1.5031580429496335E-3</v>
-      </c>
-      <c r="G21" s="1">
+        <v>-3.0452526425627305E-3</v>
+      </c>
+      <c r="G21" s="6">
         <v>-0.13614854729127701</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="2"/>
-        <v>-1.2738511589531674E-2</v>
-      </c>
-      <c r="I21" s="1">
+        <v>-2.5806990996246896E-2</v>
+      </c>
+      <c r="I21" s="6">
         <v>0.49173481421237403</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="3"/>
-        <v>4.6008347165242665E-2</v>
+        <v>9.3208456317718888E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1">
-        <v>7.5950574501408602E-2</v>
-      </c>
-      <c r="C22" s="1">
+        <v>9.3563330957023197E-2</v>
+      </c>
+      <c r="C22" s="6">
         <v>0.155274926319831</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>1.1793219859655056E-2</v>
-      </c>
-      <c r="E22" s="1">
+        <v>1.452803932058974E-2</v>
+      </c>
+      <c r="E22" s="6">
         <v>7.6795901581319298E-2</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="1"/>
-        <v>5.8326928444548337E-3</v>
-      </c>
-      <c r="G22" s="1">
+        <v>7.1852803557959583E-3</v>
+      </c>
+      <c r="G22" s="6">
         <v>0.48860184049323102</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="2"/>
-        <v>3.7109590487906505E-2</v>
-      </c>
-      <c r="I22" s="1">
+        <v>4.5715215708278835E-2</v>
+      </c>
+      <c r="I22" s="6">
         <v>-0.16340222424883499</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" si="3"/>
-        <v>-1.2410492806507018E-2</v>
+        <v>-1.5288456386507469E-2</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1">
-        <v>8.7446476159795394E-3</v>
-      </c>
-      <c r="C23" s="1">
+        <v>7.5950574501408602E-2</v>
+      </c>
+      <c r="C23" s="6">
         <v>0.13595178673816999</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>1.1888504677880969E-3</v>
-      </c>
-      <c r="E23" s="1">
+        <v>1.0325616307256993E-2</v>
+      </c>
+      <c r="E23" s="6">
         <v>7.9016118888768902E-2</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="1"/>
-        <v>6.9096811566462884E-4</v>
-      </c>
-      <c r="G23" s="1">
+        <v>6.0013196244736019E-3</v>
+      </c>
+      <c r="G23" s="6">
         <v>2.2351044704500202E-2</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="2"/>
-        <v>1.954520097898598E-4</v>
-      </c>
-      <c r="I23" s="1">
+        <v>1.6975746860134568E-3</v>
+      </c>
+      <c r="I23" s="6">
         <v>5.9314756253399097E-2</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="3"/>
-        <v>5.186866418636939E-4</v>
+        <v>4.50498981385668E-3</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1">
-        <v>-4.0838460370251399E-2</v>
-      </c>
-      <c r="C24" s="1">
+        <v>8.7446476159795394E-3</v>
+      </c>
+      <c r="C24" s="6">
         <v>-2.0936060069464399E-2</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>8.5499645945602456E-4</v>
-      </c>
-      <c r="E24" s="1">
+        <v>-1.8307846777444628E-4</v>
+      </c>
+      <c r="E24" s="6">
         <v>-1.8431666280027102E-2</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="1"/>
-        <v>7.5272087293458585E-4</v>
-      </c>
-      <c r="G24" s="1">
+        <v>-1.6117842659416946E-4</v>
+      </c>
+      <c r="G24" s="6">
         <v>-4.7356272660931099E-2</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="2"/>
-        <v>1.9339572643462546E-3</v>
-      </c>
-      <c r="I24" s="1">
+        <v>-4.1411391682608816E-4</v>
+      </c>
+      <c r="I24" s="6">
         <v>0.23567857275686899</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="3"/>
-        <v>-9.6247500536488055E-3</v>
+        <v>2.0609260693958149E-3</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1">
-        <v>-5.4341922177088102E-2</v>
-      </c>
-      <c r="C25" s="1">
+        <v>-4.0838460370251399E-2</v>
+      </c>
+      <c r="C25" s="6">
         <v>-2.4135035940555698E-2</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="0"/>
-        <v>1.3115442448229022E-3</v>
-      </c>
-      <c r="E25" s="1">
+        <v>9.8563770879297715E-4</v>
+      </c>
+      <c r="E25" s="6">
         <v>1.2336262467407299E-2</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="1"/>
-        <v>-6.7037621495998035E-4</v>
-      </c>
-      <c r="G25" s="1">
+        <v>-5.0379396589223273E-4</v>
+      </c>
+      <c r="G25" s="6">
         <v>-0.155694475159565</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="2"/>
-        <v>8.4607370525236585E-3</v>
-      </c>
-      <c r="I25" s="1">
+        <v>6.3583226536709858E-3</v>
+      </c>
+      <c r="I25" s="6">
         <v>0.219261106408184</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="3"/>
-        <v>-1.1915069980895768E-2</v>
+        <v>-8.9542860047880975E-3</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1">
-        <v>-0.118405673666667</v>
-      </c>
-      <c r="C26" s="1">
+        <v>-5.4341922177088102E-2</v>
+      </c>
+      <c r="C26" s="6">
         <v>7.0390689019331307E-2</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
-        <v>-8.3346569531947828E-3</v>
-      </c>
-      <c r="E26" s="1">
+        <v>-3.8251653446801119E-3</v>
+      </c>
+      <c r="E26" s="6">
         <v>4.92633182628677E-2</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="1"/>
-        <v>-5.8330563859702693E-3</v>
-      </c>
-      <c r="G26" s="1">
+        <v>-2.6770634072258797E-3</v>
+      </c>
+      <c r="G26" s="6">
         <v>-0.29847911239879199</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" si="2"/>
-        <v>3.5341620379007788E-2</v>
-      </c>
-      <c r="I26" s="1">
+        <v>1.6219928697461486E-2</v>
+      </c>
+      <c r="I26" s="6">
         <v>0.26199202766222202</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" si="3"/>
-        <v>-3.1021342530641455E-2</v>
+        <v>-1.4237150378237981E-2</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1">
-        <v>-0.14186323657334199</v>
-      </c>
-      <c r="C27" s="1">
+        <v>-0.118405673666667</v>
+      </c>
+      <c r="C27" s="6">
         <v>-5.5005791317053798E-2</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
-        <v>7.8032995865150835E-3</v>
-      </c>
-      <c r="E27" s="1">
+        <v>6.5129977764638572E-3</v>
+      </c>
+      <c r="E27" s="6">
         <v>-7.7744637594259397E-2</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="1"/>
-        <v>1.1029105915343158E-2</v>
-      </c>
-      <c r="G27" s="1">
+        <v>9.2054061883191686E-3</v>
+      </c>
+      <c r="G27" s="6">
         <v>0.16763128301147401</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" si="2"/>
-        <v>-2.3780716358949582E-2</v>
-      </c>
-      <c r="I27" s="1">
+        <v>-1.9848494992581293E-2</v>
+      </c>
+      <c r="I27" s="6">
         <v>0.29122653942061499</v>
       </c>
       <c r="J27" s="1">
         <f t="shared" si="3"/>
-        <v>-4.1314339458262413E-2</v>
+        <v>-3.4482874589710069E-2</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1">
-        <v>-0.18770853071708701</v>
-      </c>
-      <c r="C28" s="1">
+        <v>-0.14186323657334199</v>
+      </c>
+      <c r="C28" s="6">
         <v>-8.0764432223475804E-2</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
-        <v>1.5160172906868399E-2</v>
-      </c>
-      <c r="E28" s="1">
+        <v>1.1457503755230592E-2</v>
+      </c>
+      <c r="E28" s="6">
         <v>-4.6200392185810103E-2</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="1"/>
-        <v>8.6722077357516032E-3</v>
-      </c>
-      <c r="G28" s="1">
+        <v>6.5541371664367592E-3</v>
+      </c>
+      <c r="G28" s="6">
         <v>9.3033207687111E-2</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" si="2"/>
-        <v>-1.746312672284521E-2</v>
-      </c>
-      <c r="I28" s="1">
+        <v>-1.3197991951293486E-2</v>
+      </c>
+      <c r="I28" s="6">
         <v>0.14344114408249201</v>
       </c>
       <c r="J28" s="1">
         <f t="shared" si="3"/>
-        <v>-2.6925126400102556E-2</v>
+        <v>-2.0349024957325396E-2</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1">
-        <v>-0.23305818910992199</v>
-      </c>
-      <c r="C29" s="1">
+        <v>-0.18770853071708701</v>
+      </c>
+      <c r="C29" s="6">
         <v>2.3673681332949101E-2</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
-        <v>-5.5173453010224811E-3</v>
-      </c>
-      <c r="E29" s="1">
+        <v>-4.443751939672406E-3</v>
+      </c>
+      <c r="E29" s="6">
         <v>-3.64708065914E-2</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="1"/>
-        <v>8.4998201395698903E-3</v>
-      </c>
-      <c r="G29" s="1">
+        <v>6.8458815193387463E-3</v>
+      </c>
+      <c r="G29" s="6">
         <v>0.26082061069911999</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" si="2"/>
-        <v>-6.0786379212080847E-2</v>
-      </c>
-      <c r="I29" s="1">
+        <v>-4.8958253615065159E-2</v>
+      </c>
+      <c r="I29" s="6">
         <v>8.0683677828748898E-2</v>
       </c>
       <c r="J29" s="1">
         <f t="shared" si="3"/>
-        <v>-1.8803991845496582E-2</v>
+        <v>-1.5145014618085265E-2</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1">
-        <v>-0.25728690053321002</v>
-      </c>
-      <c r="C30" s="1">
+        <v>-0.23305818910992199</v>
+      </c>
+      <c r="C30" s="6">
         <v>-0.194348627325236</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
-        <v>5.0003355947393899E-2</v>
-      </c>
-      <c r="E30" s="1">
+        <v>4.5294539140418602E-2</v>
+      </c>
+      <c r="E30" s="6">
         <v>-0.15768584540357999</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="1"/>
-        <v>4.0570502421846018E-2</v>
-      </c>
-      <c r="G30" s="1">
+        <v>3.6749977578025471E-2</v>
+      </c>
+      <c r="G30" s="6">
         <v>-0.27364538574470798</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" si="2"/>
-        <v>7.0405373143470562E-2</v>
-      </c>
-      <c r="I30" s="1">
+        <v>6.3775298059947708E-2</v>
+      </c>
+      <c r="I30" s="6">
         <v>0.152242827588774</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" si="3"/>
-        <v>-3.9170085238727538E-2</v>
+        <v>-3.5481437702813742E-2</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1">
-        <v>-0.26797090782933303</v>
-      </c>
-      <c r="C31" s="1">
+        <v>-0.25728690053321002</v>
+      </c>
+      <c r="C31" s="6">
         <v>0.123128878902176</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
-        <v>-3.2994957459424115E-2</v>
-      </c>
-      <c r="E31" s="1">
+        <v>-3.1679447618869816E-2</v>
+      </c>
+      <c r="E31" s="6">
         <v>1.9805593236096201E-2</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="1"/>
-        <v>-5.3073227995751966E-3</v>
-      </c>
-      <c r="G31" s="1">
+        <v>-5.0957196969367005E-3</v>
+      </c>
+      <c r="G31" s="6">
         <v>3.6262863143702299E-2</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" si="2"/>
-        <v>-9.7173923571087662E-3</v>
-      </c>
-      <c r="I31" s="1">
+        <v>-9.3299596627031411E-3</v>
+      </c>
+      <c r="I31" s="6">
         <v>-1.7424115844522501E-2</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" si="3"/>
-        <v>4.6691561409801605E-3</v>
+        <v>4.4829967601687894E-3</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1">
-        <v>-0.301590012783648</v>
-      </c>
-      <c r="C32" s="1">
+        <v>-0.26797090782933303</v>
+      </c>
+      <c r="C32" s="6">
         <v>0.431717399269961</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="0"/>
-        <v>-0.13020165596475081</v>
-      </c>
-      <c r="E32" s="1">
+        <v>-0.11568770340809008</v>
+      </c>
+      <c r="E32" s="6">
         <v>0.25767423225776898</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="1"/>
-        <v>-7.7711975000637229E-2</v>
-      </c>
-      <c r="G32" s="1">
+        <v>-6.9049197942340768E-2</v>
+      </c>
+      <c r="G32" s="6">
         <v>0.273606435932161</v>
       </c>
       <c r="H32" s="1">
         <f t="shared" si="2"/>
-        <v>-8.2516968510468802E-2</v>
-      </c>
-      <c r="I32" s="1">
+        <v>-7.3318565024689433E-2</v>
+      </c>
+      <c r="I32" s="6">
         <v>-9.5504462796263803E-2</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="3"/>
-        <v>2.8803192155620636E-2</v>
+        <v>2.5592417597267571E-2</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1">
-        <v>-0.35000751131039898</v>
-      </c>
-      <c r="C33" s="1">
+        <v>-0.301590012783648</v>
+      </c>
+      <c r="C33" s="6">
         <v>3.39205988870021E-2</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="0"/>
-        <v>-1.1872464398597895E-2</v>
-      </c>
-      <c r="E33" s="1">
+        <v>-1.023011385195996E-2</v>
+      </c>
+      <c r="E33" s="6">
         <v>1.37314465719767E-2</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="1"/>
-        <v>-4.8061094413492742E-3</v>
-      </c>
-      <c r="G33" s="1">
+        <v>-4.1412671471804325E-3</v>
+      </c>
+      <c r="G33" s="6">
         <v>0.15262890948317401</v>
       </c>
       <c r="H33" s="1">
         <f t="shared" si="2"/>
-        <v>-5.342126476222589E-2</v>
-      </c>
-      <c r="I33" s="1">
+        <v>-4.6031354762184701E-2</v>
+      </c>
+      <c r="I33" s="6">
         <v>5.2564825626618003E-2</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="3"/>
-        <v>-1.839808380003765E-2</v>
+        <v>-1.585302643270195E-2</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="1">
-        <v>-0.35830110192370201</v>
-      </c>
-      <c r="C34" s="1">
+        <v>-0.35000751131039898</v>
+      </c>
+      <c r="C34" s="6">
         <v>4.5005885887476699E-2</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
-        <v>-1.612565850653529E-2</v>
-      </c>
-      <c r="E34" s="1">
+        <v>-1.5752398113795526E-2</v>
+      </c>
+      <c r="E34" s="6">
         <v>8.8953563741296492E-3</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="1"/>
-        <v>-3.1872159908546797E-3</v>
-      </c>
-      <c r="G34" s="1">
+        <v>-3.1134415467282128E-3</v>
+      </c>
+      <c r="G34" s="6">
         <v>-5.2204564884948998E-2</v>
       </c>
       <c r="H34" s="1">
         <f t="shared" si="2"/>
-        <v>1.8704953123724628E-2</v>
-      </c>
-      <c r="I34" s="1">
+        <v>1.8271989834423245E-2</v>
+      </c>
+      <c r="I34" s="6">
         <v>9.5703993034089802E-2</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="3"/>
-        <v>-3.429084616261268E-2</v>
+        <v>-3.349711642432953E-2</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2018,22 +2035,22 @@
       <c r="C35" s="2"/>
       <c r="D35" s="2">
         <f>SUM(D3:D34)</f>
-        <v>0.79106619243983256</v>
+        <v>8.7703116033379533E-2</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2">
         <f>SUM(F3:F34)</f>
-        <v>1.2592555268948857</v>
+        <v>0.74639468174968882</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2">
         <f>SUM(H3:H34)</f>
-        <v>1.4999307447254442</v>
+        <v>0.99587632615337607</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2">
         <f>SUM(J3:J34)</f>
-        <v>1.7991337495452717</v>
+        <v>-0.25402789501316753</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -2044,22 +2061,22 @@
       <c r="C36" s="2"/>
       <c r="D36" s="2">
         <f>MAX(MIN(1,D35),0)</f>
-        <v>0.79106619243983256</v>
+        <v>8.7703116033379533E-2</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2">
         <f>MAX(MIN(1,F35),0)</f>
-        <v>1</v>
+        <v>0.74639468174968882</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2">
         <f>MAX(MIN(1,H35),0)</f>
-        <v>1</v>
+        <v>0.99587632615337607</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2">
         <f>MAX(MIN(1,J35),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2076,53 +2093,53 @@
     <row r="39" spans="1:10">
       <c r="B39" s="1">
         <f>D36</f>
-        <v>0.79106619243983256</v>
+        <v>8.7703116033379533E-2</v>
       </c>
       <c r="C39" s="1">
         <v>-1.9716240819995401</v>
       </c>
       <c r="D39" s="1">
         <f>B39*C39</f>
-        <v>-1.5596851554700564</v>
+        <v>-0.17291757563781107</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="B40" s="1">
         <f>F36</f>
-        <v>1</v>
+        <v>0.74639468174968882</v>
       </c>
       <c r="C40" s="1">
         <v>1.95869794985069</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" ref="D40:D42" si="4">B40*C40</f>
-        <v>1.95869794985069</v>
+        <v>1.4619617329225738</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="B41" s="1">
         <f>H36</f>
-        <v>1</v>
+        <v>0.99587632615337607</v>
       </c>
       <c r="C41" s="1">
         <v>9.1621721193967099E-4</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" si="4"/>
-        <v>9.1621721193967099E-4</v>
+        <v>9.1243903098496863E-4</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="B42" s="1">
         <f>J36</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" s="1">
         <v>-1.0954085028823</v>
       </c>
       <c r="D42" s="1">
         <f t="shared" si="4"/>
-        <v>-1.0954085028823</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2132,7 +2149,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3">
         <f>SUM(D39:D42)</f>
-        <v>-0.69547949128972664</v>
+        <v>1.2899565963157476</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2142,7 +2159,7 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3">
         <f>MAX(MIN(D43,1),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>